<commit_message>
normal version after valentine
</commit_message>
<xml_diff>
--- a/google/shedule.xlsx
+++ b/google/shedule.xlsx
@@ -11,7 +11,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="52" uniqueCount="23">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="56" uniqueCount="29">
   <si>
     <t>Расписание стримов</t>
   </si>
@@ -37,19 +37,37 @@
     <t>Озвучка/Сабы</t>
   </si>
   <si>
+    <t>290166276796448768</t>
+  </si>
+  <si>
+    <t>Initial D</t>
+  </si>
+  <si>
+    <t>с 1 серии примерно 7-8, как пойдёт</t>
+  </si>
+  <si>
+    <t>Сабы &lt;:YEP:771044606913151002&gt;</t>
+  </si>
+  <si>
     <t>793963638901833769</t>
   </si>
   <si>
-    <t>Гуррен-Лаганн</t>
-  </si>
-  <si>
-    <t>с 22 до конца</t>
-  </si>
-  <si>
     <t>Обан: Звездные гонки</t>
   </si>
   <si>
     <t>с 1 по 7</t>
+  </si>
+  <si>
+    <t>Озвучка</t>
+  </si>
+  <si>
+    <t>Гинтама</t>
+  </si>
+  <si>
+    <t>с 17 по 32</t>
+  </si>
+  <si>
+    <t>Animedia</t>
   </si>
   <si>
     <t>с 8 по 14</t>
@@ -128,7 +146,7 @@
   <cellStyleXfs count="1">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" applyAlignment="1" applyFont="1"/>
   </cellStyleXfs>
-  <cellXfs count="13">
+  <cellXfs count="12">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
     </xf>
@@ -147,26 +165,23 @@
     <xf borderId="0" fillId="0" fontId="2" numFmtId="164" xfId="0" applyAlignment="1" applyFont="1" applyNumberFormat="1">
       <alignment readingOrder="0" vertical="bottom"/>
     </xf>
-    <xf borderId="0" fillId="0" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment vertical="bottom"/>
-    </xf>
     <xf borderId="0" fillId="2" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyFill="1" applyFont="1">
       <alignment readingOrder="0" vertical="bottom"/>
     </xf>
+    <xf borderId="0" fillId="0" fontId="4" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment readingOrder="0"/>
+    </xf>
+    <xf borderId="0" fillId="0" fontId="1" numFmtId="20" xfId="0" applyAlignment="1" applyFont="1" applyNumberFormat="1">
+      <alignment readingOrder="0"/>
+    </xf>
+    <xf borderId="0" fillId="0" fontId="4" numFmtId="20" xfId="0" applyAlignment="1" applyFont="1" applyNumberFormat="1">
+      <alignment readingOrder="0"/>
+    </xf>
     <xf borderId="0" fillId="0" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0" vertical="bottom"/>
     </xf>
-    <xf borderId="0" fillId="0" fontId="4" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment readingOrder="0"/>
-    </xf>
-    <xf borderId="0" fillId="0" fontId="4" numFmtId="20" xfId="0" applyAlignment="1" applyFont="1" applyNumberFormat="1">
-      <alignment readingOrder="0"/>
-    </xf>
     <xf borderId="0" fillId="0" fontId="1" numFmtId="164" xfId="0" applyAlignment="1" applyFont="1" applyNumberFormat="1">
       <alignment readingOrder="0" vertical="bottom"/>
-    </xf>
-    <xf borderId="0" fillId="0" fontId="1" numFmtId="20" xfId="0" applyAlignment="1" applyFont="1" applyNumberFormat="1">
-      <alignment readingOrder="0"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -433,341 +448,360 @@
     </row>
     <row r="4">
       <c r="B4" s="5">
-        <v>44235.0</v>
-      </c>
-      <c r="D4" s="6"/>
+        <v>44238.0</v>
+      </c>
     </row>
     <row r="5">
       <c r="A5" s="1"/>
-      <c r="D5" s="7" t="s">
+      <c r="D5" s="6" t="s">
         <v>8</v>
       </c>
-      <c r="E5" s="8" t="s">
+      <c r="E5" s="7" t="s">
         <v>9</v>
       </c>
-      <c r="F5" s="9" t="s">
+      <c r="F5" s="7" t="s">
         <v>10</v>
       </c>
-      <c r="G5" s="10">
-        <v>0.8958333333333334</v>
-      </c>
-      <c r="H5" s="9">
-        <v>1.0</v>
-      </c>
-      <c r="I5" s="4" t="s">
-        <v>7</v>
+      <c r="G5" s="8">
+        <v>0.8958333333333334</v>
+      </c>
+      <c r="H5" s="7">
+        <v>1.0</v>
+      </c>
+      <c r="I5" s="7" t="s">
+        <v>11</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" s="2"/>
+      <c r="D6" s="6"/>
+      <c r="G6" s="9"/>
     </row>
     <row r="7">
       <c r="A7" s="1"/>
-      <c r="B7" s="11">
-        <v>44237.0</v>
-      </c>
+      <c r="B7" s="5">
+        <v>44239.0</v>
+      </c>
+      <c r="D7" s="2"/>
     </row>
     <row r="8">
       <c r="A8" s="1"/>
-      <c r="D8" s="7" t="s">
-        <v>8</v>
-      </c>
-      <c r="E8" s="9" t="s">
-        <v>11</v>
-      </c>
-      <c r="F8" s="9" t="s">
-        <v>12</v>
-      </c>
-      <c r="G8" s="10">
-        <v>0.8958333333333334</v>
-      </c>
-      <c r="H8" s="4">
-        <v>1.0</v>
-      </c>
-      <c r="I8" s="4" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="9">
-      <c r="D9" s="7"/>
-      <c r="G9" s="12"/>
+      <c r="D8" s="6" t="s">
+        <v>12</v>
+      </c>
+      <c r="E8" s="7" t="s">
+        <v>13</v>
+      </c>
+      <c r="F8" s="7" t="s">
+        <v>14</v>
+      </c>
+      <c r="G8" s="9">
+        <v>0.8958333333333334</v>
+      </c>
+      <c r="H8" s="7">
+        <v>1.0</v>
+      </c>
+      <c r="I8" s="7" t="s">
+        <v>15</v>
+      </c>
     </row>
     <row r="10">
       <c r="A10" s="1"/>
-      <c r="B10" s="11">
-        <v>44239.0</v>
-      </c>
-      <c r="D10" s="6"/>
+      <c r="B10" s="5">
+        <v>44241.0</v>
+      </c>
+      <c r="D10" s="2"/>
     </row>
     <row r="11">
       <c r="A11" s="1"/>
-      <c r="D11" s="7" t="s">
-        <v>8</v>
-      </c>
-      <c r="E11" s="4" t="s">
-        <v>11</v>
-      </c>
-      <c r="F11" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="G11" s="10">
-        <v>0.8958333333333334</v>
+      <c r="D11" s="6" t="s">
+        <v>12</v>
+      </c>
+      <c r="E11" s="7" t="s">
+        <v>16</v>
+      </c>
+      <c r="F11" s="7" t="s">
+        <v>17</v>
+      </c>
+      <c r="G11" s="9">
+        <v>0.6666666666666666</v>
       </c>
       <c r="H11" s="4">
         <v>1.0</v>
       </c>
-      <c r="I11" s="4" t="s">
-        <v>7</v>
+      <c r="I11" s="7" t="s">
+        <v>18</v>
       </c>
     </row>
     <row r="13">
       <c r="A13" s="1"/>
-      <c r="B13" s="11">
+      <c r="B13" s="5">
         <v>44242.0</v>
       </c>
     </row>
     <row r="14">
-      <c r="D14" s="7" t="s">
-        <v>8</v>
-      </c>
-      <c r="E14" s="9" t="s">
-        <v>11</v>
-      </c>
-      <c r="F14" s="9" t="s">
-        <v>14</v>
-      </c>
-      <c r="G14" s="10">
-        <v>0.8958333333333334</v>
-      </c>
-      <c r="H14" s="9">
-        <v>1.0</v>
-      </c>
-      <c r="I14" s="9" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="15">
-      <c r="D15" s="7"/>
-      <c r="G15" s="12"/>
+      <c r="D14" s="6" t="s">
+        <v>12</v>
+      </c>
+      <c r="E14" s="7" t="s">
+        <v>13</v>
+      </c>
+      <c r="F14" s="10" t="s">
+        <v>19</v>
+      </c>
+      <c r="G14" s="9">
+        <v>0.8958333333333334</v>
+      </c>
+      <c r="H14" s="7">
+        <v>1.0</v>
+      </c>
+      <c r="I14" s="7" t="s">
+        <v>15</v>
+      </c>
     </row>
     <row r="16">
       <c r="A16" s="1"/>
       <c r="B16" s="5">
         <v>44244.0</v>
       </c>
-      <c r="D16" s="2"/>
     </row>
     <row r="17">
-      <c r="D17" s="7" t="s">
-        <v>8</v>
-      </c>
-      <c r="E17" s="9" t="s">
-        <v>11</v>
-      </c>
-      <c r="F17" s="9" t="s">
+      <c r="D17" s="6" t="s">
+        <v>12</v>
+      </c>
+      <c r="E17" s="7" t="s">
+        <v>13</v>
+      </c>
+      <c r="F17" s="7" t="s">
+        <v>20</v>
+      </c>
+      <c r="G17" s="9">
+        <v>0.8958333333333334</v>
+      </c>
+      <c r="H17" s="7">
+        <v>1.0</v>
+      </c>
+      <c r="I17" s="7" t="s">
         <v>15</v>
       </c>
-      <c r="G17" s="10">
-        <v>0.8958333333333334</v>
-      </c>
-      <c r="H17" s="9">
-        <v>1.0</v>
-      </c>
-      <c r="I17" s="9" t="s">
-        <v>7</v>
-      </c>
+    </row>
+    <row r="18">
+      <c r="D18" s="6"/>
+      <c r="G18" s="8"/>
     </row>
     <row r="19">
       <c r="A19" s="1"/>
       <c r="B19" s="5">
         <v>44246.0</v>
       </c>
+      <c r="D19" s="2"/>
     </row>
     <row r="20">
-      <c r="D20" s="7" t="s">
-        <v>8</v>
-      </c>
-      <c r="E20" s="9" t="s">
-        <v>16</v>
-      </c>
-      <c r="F20" s="9" t="s">
-        <v>17</v>
-      </c>
-      <c r="G20" s="10">
-        <v>0.8958333333333334</v>
-      </c>
-      <c r="H20" s="9">
-        <v>1.0</v>
-      </c>
-      <c r="I20" s="9" t="s">
-        <v>7</v>
+      <c r="D20" s="6" t="s">
+        <v>12</v>
+      </c>
+      <c r="E20" s="7" t="s">
+        <v>13</v>
+      </c>
+      <c r="F20" s="7" t="s">
+        <v>21</v>
+      </c>
+      <c r="G20" s="9">
+        <v>0.8958333333333334</v>
+      </c>
+      <c r="H20" s="7">
+        <v>1.0</v>
+      </c>
+      <c r="I20" s="7" t="s">
+        <v>15</v>
       </c>
     </row>
     <row r="21">
-      <c r="B21" s="11"/>
-      <c r="D21" s="7"/>
-      <c r="G21" s="12"/>
+      <c r="B21" s="5"/>
     </row>
     <row r="22">
       <c r="A22" s="1"/>
       <c r="B22" s="5">
         <v>44249.0</v>
       </c>
-      <c r="D22" s="2"/>
     </row>
     <row r="23">
-      <c r="D23" s="7" t="s">
-        <v>8</v>
-      </c>
-      <c r="E23" s="9" t="s">
-        <v>16</v>
-      </c>
-      <c r="F23" s="8" t="s">
-        <v>18</v>
-      </c>
-      <c r="G23" s="10">
-        <v>0.8958333333333334</v>
-      </c>
-      <c r="H23" s="9">
-        <v>1.0</v>
-      </c>
-      <c r="I23" s="9" t="s">
+      <c r="D23" s="6" t="s">
+        <v>12</v>
+      </c>
+      <c r="E23" s="7" t="s">
+        <v>22</v>
+      </c>
+      <c r="F23" s="7" t="s">
+        <v>23</v>
+      </c>
+      <c r="G23" s="9">
+        <v>0.8958333333333334</v>
+      </c>
+      <c r="H23" s="7">
+        <v>1.0</v>
+      </c>
+      <c r="I23" s="7" t="s">
         <v>7</v>
       </c>
     </row>
     <row r="24">
       <c r="A24" s="1"/>
       <c r="B24" s="11"/>
+      <c r="D24" s="6"/>
+      <c r="G24" s="8"/>
     </row>
     <row r="25">
       <c r="A25" s="1"/>
       <c r="B25" s="5">
         <v>44251.0</v>
       </c>
+      <c r="D25" s="2"/>
     </row>
     <row r="26">
-      <c r="D26" s="7" t="s">
-        <v>8</v>
-      </c>
-      <c r="E26" s="9" t="s">
-        <v>19</v>
-      </c>
-      <c r="F26" s="9" t="s">
-        <v>17</v>
-      </c>
-      <c r="G26" s="10">
-        <v>0.8958333333333334</v>
-      </c>
-      <c r="H26" s="9">
-        <v>1.0</v>
-      </c>
-      <c r="I26" s="9" t="s">
+      <c r="D26" s="6" t="s">
+        <v>12</v>
+      </c>
+      <c r="E26" s="7" t="s">
+        <v>22</v>
+      </c>
+      <c r="F26" s="10" t="s">
+        <v>24</v>
+      </c>
+      <c r="G26" s="9">
+        <v>0.8958333333333334</v>
+      </c>
+      <c r="H26" s="7">
+        <v>1.0</v>
+      </c>
+      <c r="I26" s="7" t="s">
         <v>7</v>
       </c>
     </row>
     <row r="27">
       <c r="A27" s="1"/>
-      <c r="D27" s="7"/>
-      <c r="G27" s="12"/>
     </row>
     <row r="28">
       <c r="A28" s="1"/>
       <c r="B28" s="5">
         <v>44253.0</v>
       </c>
-      <c r="D28" s="1"/>
     </row>
     <row r="29">
       <c r="A29" s="1"/>
-      <c r="D29" s="7" t="s">
-        <v>8</v>
-      </c>
-      <c r="E29" s="9" t="s">
-        <v>19</v>
-      </c>
-      <c r="F29" s="8" t="s">
-        <v>20</v>
-      </c>
-      <c r="G29" s="10">
-        <v>0.8958333333333334</v>
-      </c>
-      <c r="H29" s="9">
-        <v>1.0</v>
-      </c>
-      <c r="I29" s="9" t="s">
+      <c r="D29" s="6" t="s">
+        <v>12</v>
+      </c>
+      <c r="E29" s="7" t="s">
+        <v>25</v>
+      </c>
+      <c r="F29" s="7" t="s">
+        <v>23</v>
+      </c>
+      <c r="G29" s="9">
+        <v>0.8958333333333334</v>
+      </c>
+      <c r="H29" s="7">
+        <v>1.0</v>
+      </c>
+      <c r="I29" s="7" t="s">
         <v>7</v>
       </c>
     </row>
     <row r="30">
       <c r="B30" s="5"/>
+      <c r="D30" s="6"/>
+      <c r="G30" s="8"/>
     </row>
     <row r="31">
       <c r="A31" s="1"/>
       <c r="B31" s="5">
         <v>44256.0</v>
       </c>
+      <c r="D31" s="1"/>
     </row>
     <row r="32">
       <c r="A32" s="1"/>
-      <c r="D32" s="7" t="s">
-        <v>8</v>
-      </c>
-      <c r="E32" s="9" t="s">
-        <v>19</v>
-      </c>
-      <c r="F32" s="9" t="s">
-        <v>21</v>
-      </c>
-      <c r="G32" s="10">
-        <v>0.8958333333333334</v>
-      </c>
-      <c r="H32" s="9">
-        <v>1.0</v>
-      </c>
-      <c r="I32" s="9" t="s">
+      <c r="D32" s="6" t="s">
+        <v>12</v>
+      </c>
+      <c r="E32" s="7" t="s">
+        <v>25</v>
+      </c>
+      <c r="F32" s="10" t="s">
+        <v>26</v>
+      </c>
+      <c r="G32" s="9">
+        <v>0.8958333333333334</v>
+      </c>
+      <c r="H32" s="7">
+        <v>1.0</v>
+      </c>
+      <c r="I32" s="7" t="s">
         <v>7</v>
       </c>
     </row>
     <row r="33">
-      <c r="B33" s="5"/>
-      <c r="D33" s="7"/>
-      <c r="G33" s="12"/>
+      <c r="B33" s="11"/>
     </row>
     <row r="34">
       <c r="A34" s="1"/>
       <c r="B34" s="5">
         <v>44258.0</v>
       </c>
-      <c r="D34" s="2"/>
     </row>
     <row r="35">
-      <c r="D35" s="7" t="s">
-        <v>8</v>
-      </c>
-      <c r="E35" s="9" t="s">
-        <v>19</v>
-      </c>
-      <c r="F35" s="9" t="s">
-        <v>22</v>
-      </c>
-      <c r="G35" s="10">
-        <v>0.8958333333333334</v>
-      </c>
-      <c r="H35" s="9">
-        <v>1.0</v>
-      </c>
-      <c r="I35" s="9" t="s">
+      <c r="D35" s="6" t="s">
+        <v>12</v>
+      </c>
+      <c r="E35" s="7" t="s">
+        <v>25</v>
+      </c>
+      <c r="F35" s="7" t="s">
+        <v>27</v>
+      </c>
+      <c r="G35" s="9">
+        <v>0.8958333333333334</v>
+      </c>
+      <c r="H35" s="7">
+        <v>1.0</v>
+      </c>
+      <c r="I35" s="7" t="s">
         <v>7</v>
       </c>
     </row>
     <row r="36">
       <c r="A36" s="1"/>
+      <c r="D36" s="6"/>
+      <c r="G36" s="8"/>
     </row>
     <row r="37">
       <c r="A37" s="1"/>
+      <c r="B37" s="11">
+        <v>44260.0</v>
+      </c>
+      <c r="D37" s="2"/>
     </row>
     <row r="38">
       <c r="A38" s="1"/>
+      <c r="D38" s="6" t="s">
+        <v>12</v>
+      </c>
+      <c r="E38" s="4" t="s">
+        <v>25</v>
+      </c>
+      <c r="F38" s="4" t="s">
+        <v>28</v>
+      </c>
+      <c r="G38" s="8">
+        <v>0.8958333333333334</v>
+      </c>
+      <c r="H38" s="4">
+        <v>1.0</v>
+      </c>
+      <c r="I38" s="4" t="s">
+        <v>7</v>
+      </c>
     </row>
     <row r="39">
       <c r="A39" s="1"/>

</xml_diff>

<commit_message>
Create music player and adding split shedule
</commit_message>
<xml_diff>
--- a/google/shedule.xlsx
+++ b/google/shedule.xlsx
@@ -11,7 +11,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="56" uniqueCount="29">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="16">
   <si>
     <t>Расписание стримов</t>
   </si>
@@ -37,67 +37,28 @@
     <t>Озвучка/Сабы</t>
   </si>
   <si>
-    <t>290166276796448768</t>
-  </si>
-  <si>
-    <t>Initial D</t>
-  </si>
-  <si>
-    <t>с 1 серии примерно 7-8, как пойдёт</t>
-  </si>
-  <si>
-    <t>Сабы &lt;:YEP:771044606913151002&gt;</t>
-  </si>
-  <si>
-    <t>793963638901833769</t>
-  </si>
-  <si>
-    <t>Обан: Звездные гонки</t>
-  </si>
-  <si>
-    <t>с 1 по 7</t>
+    <t>304578501351047178</t>
+  </si>
+  <si>
+    <t>Деревенская глубинка 3</t>
+  </si>
+  <si>
+    <t>с 7 по 12</t>
+  </si>
+  <si>
+    <t>Субтитры</t>
+  </si>
+  <si>
+    <t>369138872048943115</t>
+  </si>
+  <si>
+    <t>Лагерь на свежем воздухе 2</t>
+  </si>
+  <si>
+    <t>с 1 по 6</t>
   </si>
   <si>
     <t>Озвучка</t>
-  </si>
-  <si>
-    <t>Гинтама</t>
-  </si>
-  <si>
-    <t>с 17 по 32</t>
-  </si>
-  <si>
-    <t>Animedia</t>
-  </si>
-  <si>
-    <t>с 8 по 14</t>
-  </si>
-  <si>
-    <t>с 15 по 20</t>
-  </si>
-  <si>
-    <t>с 21 до конца</t>
-  </si>
-  <si>
-    <t>История мечей</t>
-  </si>
-  <si>
-    <t>с 1 по 6</t>
-  </si>
-  <si>
-    <t>с 7 до конца</t>
-  </si>
-  <si>
-    <t>Доктор Стоун</t>
-  </si>
-  <si>
-    <t>с 7 по 12</t>
-  </si>
-  <si>
-    <t>с 13 по 18</t>
-  </si>
-  <si>
-    <t>с 19 до конца</t>
   </si>
 </sst>
 </file>
@@ -107,7 +68,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="d mmmm"/>
   </numFmts>
-  <fonts count="5">
+  <fonts count="4">
     <font>
       <sz val="10.0"/>
       <color rgb="FF000000"/>
@@ -118,13 +79,14 @@
       <name val="Arial"/>
     </font>
     <font>
-      <name val="Arial"/>
+      <sz val="10.0"/>
+      <color rgb="FF112233"/>
+      <name val="&quot;Open Sans&quot;"/>
     </font>
     <font>
       <color rgb="FF000000"/>
       <name val="Arial"/>
     </font>
-    <font/>
   </fonts>
   <fills count="3">
     <fill>
@@ -146,7 +108,7 @@
   <cellStyleXfs count="1">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" applyAlignment="1" applyFont="1"/>
   </cellStyleXfs>
-  <cellXfs count="12">
+  <cellXfs count="10">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
     </xf>
@@ -162,25 +124,19 @@
     <xf borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0"/>
     </xf>
-    <xf borderId="0" fillId="0" fontId="2" numFmtId="164" xfId="0" applyAlignment="1" applyFont="1" applyNumberFormat="1">
-      <alignment readingOrder="0" vertical="bottom"/>
-    </xf>
-    <xf borderId="0" fillId="2" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyFill="1" applyFont="1">
-      <alignment readingOrder="0" vertical="bottom"/>
-    </xf>
-    <xf borderId="0" fillId="0" fontId="4" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+    <xf borderId="0" fillId="0" fontId="1" numFmtId="164" xfId="0" applyAlignment="1" applyFont="1" applyNumberFormat="1">
       <alignment readingOrder="0"/>
     </xf>
     <xf borderId="0" fillId="0" fontId="1" numFmtId="20" xfId="0" applyAlignment="1" applyFont="1" applyNumberFormat="1">
       <alignment readingOrder="0"/>
     </xf>
-    <xf borderId="0" fillId="0" fontId="4" numFmtId="20" xfId="0" applyAlignment="1" applyFont="1" applyNumberFormat="1">
+    <xf borderId="0" fillId="2" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyFill="1" applyFont="1">
       <alignment readingOrder="0"/>
     </xf>
-    <xf borderId="0" fillId="0" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+    <xf borderId="0" fillId="0" fontId="1" numFmtId="164" xfId="0" applyAlignment="1" applyFont="1" applyNumberFormat="1">
       <alignment readingOrder="0" vertical="bottom"/>
     </xf>
-    <xf borderId="0" fillId="0" fontId="1" numFmtId="164" xfId="0" applyAlignment="1" applyFont="1" applyNumberFormat="1">
+    <xf borderId="0" fillId="2" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0" vertical="bottom"/>
     </xf>
   </cellXfs>
@@ -448,360 +404,172 @@
     </row>
     <row r="4">
       <c r="B4" s="5">
-        <v>44238.0</v>
+        <v>44295.0</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" s="1"/>
-      <c r="D5" s="6" t="s">
+      <c r="D5" s="4" t="s">
         <v>8</v>
       </c>
-      <c r="E5" s="7" t="s">
+      <c r="E5" s="4" t="s">
         <v>9</v>
       </c>
-      <c r="F5" s="7" t="s">
+      <c r="F5" s="4" t="s">
         <v>10</v>
       </c>
-      <c r="G5" s="8">
-        <v>0.8958333333333334</v>
-      </c>
-      <c r="H5" s="7">
+      <c r="G5" s="6">
+        <v>0.7916666666666666</v>
+      </c>
+      <c r="H5" s="4">
         <v>1.0</v>
       </c>
-      <c r="I5" s="7" t="s">
+      <c r="I5" s="4" t="s">
         <v>11</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" s="2"/>
-      <c r="D6" s="6"/>
-      <c r="G6" s="9"/>
     </row>
     <row r="7">
       <c r="A7" s="1"/>
       <c r="B7" s="5">
-        <v>44239.0</v>
-      </c>
-      <c r="D7" s="2"/>
+        <v>44296.0</v>
+      </c>
     </row>
     <row r="8">
       <c r="A8" s="1"/>
-      <c r="D8" s="6" t="s">
+      <c r="D8" s="4" t="s">
         <v>12</v>
       </c>
-      <c r="E8" s="7" t="s">
+      <c r="E8" s="4" t="s">
         <v>13</v>
       </c>
-      <c r="F8" s="7" t="s">
+      <c r="F8" s="4" t="s">
         <v>14</v>
       </c>
-      <c r="G8" s="9">
-        <v>0.8958333333333334</v>
-      </c>
-      <c r="H8" s="7">
+      <c r="G8" s="6">
+        <v>0.625</v>
+      </c>
+      <c r="H8" s="4">
         <v>1.0</v>
       </c>
-      <c r="I8" s="7" t="s">
+      <c r="I8" s="4" t="s">
         <v>15</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" s="1"/>
       <c r="B10" s="5">
-        <v>44241.0</v>
-      </c>
-      <c r="D10" s="2"/>
+        <v>44297.0</v>
+      </c>
     </row>
     <row r="11">
       <c r="A11" s="1"/>
-      <c r="D11" s="6" t="s">
+      <c r="D11" s="4" t="s">
         <v>12</v>
       </c>
-      <c r="E11" s="7" t="s">
-        <v>16</v>
-      </c>
-      <c r="F11" s="7" t="s">
-        <v>17</v>
-      </c>
-      <c r="G11" s="9">
-        <v>0.6666666666666666</v>
+      <c r="E11" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="F11" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="G11" s="6">
+        <v>0.625</v>
       </c>
       <c r="H11" s="4">
         <v>1.0</v>
       </c>
-      <c r="I11" s="7" t="s">
-        <v>18</v>
+      <c r="I11" s="4" t="s">
+        <v>15</v>
       </c>
     </row>
     <row r="13">
       <c r="A13" s="1"/>
-      <c r="B13" s="5">
-        <v>44242.0</v>
-      </c>
-    </row>
-    <row r="14">
-      <c r="D14" s="6" t="s">
-        <v>12</v>
-      </c>
-      <c r="E14" s="7" t="s">
-        <v>13</v>
-      </c>
-      <c r="F14" s="10" t="s">
-        <v>19</v>
-      </c>
-      <c r="G14" s="9">
-        <v>0.8958333333333334</v>
-      </c>
-      <c r="H14" s="7">
-        <v>1.0</v>
-      </c>
-      <c r="I14" s="7" t="s">
-        <v>15</v>
-      </c>
     </row>
     <row r="16">
       <c r="A16" s="1"/>
-      <c r="B16" s="5">
-        <v>44244.0</v>
-      </c>
-    </row>
-    <row r="17">
-      <c r="D17" s="6" t="s">
-        <v>12</v>
-      </c>
-      <c r="E17" s="7" t="s">
-        <v>13</v>
-      </c>
-      <c r="F17" s="7" t="s">
-        <v>20</v>
-      </c>
-      <c r="G17" s="9">
-        <v>0.8958333333333334</v>
-      </c>
-      <c r="H17" s="7">
-        <v>1.0</v>
-      </c>
-      <c r="I17" s="7" t="s">
-        <v>15</v>
-      </c>
     </row>
     <row r="18">
-      <c r="D18" s="6"/>
-      <c r="G18" s="8"/>
+      <c r="B18" s="5"/>
     </row>
     <row r="19">
       <c r="A19" s="1"/>
-      <c r="B19" s="5">
-        <v>44246.0</v>
-      </c>
-      <c r="D19" s="2"/>
+      <c r="E19" s="7"/>
+      <c r="G19" s="6"/>
     </row>
     <row r="20">
-      <c r="D20" s="6" t="s">
-        <v>12</v>
-      </c>
-      <c r="E20" s="7" t="s">
-        <v>13</v>
-      </c>
-      <c r="F20" s="7" t="s">
-        <v>21</v>
-      </c>
-      <c r="G20" s="9">
-        <v>0.8958333333333334</v>
-      </c>
-      <c r="H20" s="7">
-        <v>1.0</v>
-      </c>
-      <c r="I20" s="7" t="s">
-        <v>15</v>
-      </c>
+      <c r="E20" s="2"/>
+      <c r="F20" s="2"/>
     </row>
     <row r="21">
       <c r="B21" s="5"/>
     </row>
     <row r="22">
       <c r="A22" s="1"/>
-      <c r="B22" s="5">
-        <v>44249.0</v>
-      </c>
-    </row>
-    <row r="23">
-      <c r="D23" s="6" t="s">
-        <v>12</v>
-      </c>
-      <c r="E23" s="7" t="s">
-        <v>22</v>
-      </c>
-      <c r="F23" s="7" t="s">
-        <v>23</v>
-      </c>
-      <c r="G23" s="9">
-        <v>0.8958333333333334</v>
-      </c>
-      <c r="H23" s="7">
-        <v>1.0</v>
-      </c>
-      <c r="I23" s="7" t="s">
-        <v>7</v>
-      </c>
+      <c r="E22" s="7"/>
+      <c r="G22" s="6"/>
     </row>
     <row r="24">
       <c r="A24" s="1"/>
-      <c r="B24" s="11"/>
-      <c r="D24" s="6"/>
-      <c r="G24" s="8"/>
     </row>
     <row r="25">
       <c r="A25" s="1"/>
-      <c r="B25" s="5">
-        <v>44251.0</v>
-      </c>
-      <c r="D25" s="2"/>
-    </row>
-    <row r="26">
-      <c r="D26" s="6" t="s">
-        <v>12</v>
-      </c>
-      <c r="E26" s="7" t="s">
-        <v>22</v>
-      </c>
-      <c r="F26" s="10" t="s">
-        <v>24</v>
-      </c>
-      <c r="G26" s="9">
-        <v>0.8958333333333334</v>
-      </c>
-      <c r="H26" s="7">
-        <v>1.0</v>
-      </c>
-      <c r="I26" s="7" t="s">
-        <v>7</v>
-      </c>
     </row>
     <row r="27">
       <c r="A27" s="1"/>
     </row>
     <row r="28">
       <c r="A28" s="1"/>
-      <c r="B28" s="5">
-        <v>44253.0</v>
-      </c>
+      <c r="B28" s="8"/>
     </row>
     <row r="29">
       <c r="A29" s="1"/>
-      <c r="D29" s="6" t="s">
-        <v>12</v>
-      </c>
-      <c r="E29" s="7" t="s">
-        <v>25</v>
-      </c>
-      <c r="F29" s="7" t="s">
-        <v>23</v>
-      </c>
-      <c r="G29" s="9">
-        <v>0.8958333333333334</v>
-      </c>
-      <c r="H29" s="7">
-        <v>1.0</v>
-      </c>
-      <c r="I29" s="7" t="s">
-        <v>7</v>
-      </c>
+      <c r="D29" s="9"/>
+      <c r="G29" s="6"/>
     </row>
     <row r="30">
-      <c r="B30" s="5"/>
-      <c r="D30" s="6"/>
-      <c r="G30" s="8"/>
+      <c r="B30" s="8"/>
+      <c r="D30" s="9"/>
+      <c r="G30" s="6"/>
     </row>
     <row r="31">
       <c r="A31" s="1"/>
-      <c r="B31" s="5">
-        <v>44256.0</v>
-      </c>
+      <c r="B31" s="8"/>
       <c r="D31" s="1"/>
     </row>
     <row r="32">
       <c r="A32" s="1"/>
-      <c r="D32" s="6" t="s">
-        <v>12</v>
-      </c>
-      <c r="E32" s="7" t="s">
-        <v>25</v>
-      </c>
-      <c r="F32" s="10" t="s">
-        <v>26</v>
-      </c>
-      <c r="G32" s="9">
-        <v>0.8958333333333334</v>
-      </c>
-      <c r="H32" s="7">
-        <v>1.0</v>
-      </c>
-      <c r="I32" s="7" t="s">
-        <v>7</v>
-      </c>
+      <c r="D32" s="9"/>
+      <c r="F32" s="1"/>
+      <c r="G32" s="6"/>
     </row>
     <row r="33">
-      <c r="B33" s="11"/>
+      <c r="B33" s="8"/>
     </row>
     <row r="34">
       <c r="A34" s="1"/>
-      <c r="B34" s="5">
-        <v>44258.0</v>
-      </c>
+      <c r="B34" s="8"/>
     </row>
     <row r="35">
-      <c r="D35" s="6" t="s">
-        <v>12</v>
-      </c>
-      <c r="E35" s="7" t="s">
-        <v>25</v>
-      </c>
-      <c r="F35" s="7" t="s">
-        <v>27</v>
-      </c>
-      <c r="G35" s="9">
-        <v>0.8958333333333334</v>
-      </c>
-      <c r="H35" s="7">
-        <v>1.0</v>
-      </c>
-      <c r="I35" s="7" t="s">
-        <v>7</v>
-      </c>
+      <c r="D35" s="9"/>
+      <c r="G35" s="6"/>
     </row>
     <row r="36">
       <c r="A36" s="1"/>
-      <c r="D36" s="6"/>
-      <c r="G36" s="8"/>
+      <c r="D36" s="9"/>
+      <c r="G36" s="6"/>
     </row>
     <row r="37">
       <c r="A37" s="1"/>
-      <c r="B37" s="11">
-        <v>44260.0</v>
-      </c>
+      <c r="B37" s="8"/>
       <c r="D37" s="2"/>
     </row>
     <row r="38">
       <c r="A38" s="1"/>
-      <c r="D38" s="6" t="s">
-        <v>12</v>
-      </c>
-      <c r="E38" s="4" t="s">
-        <v>25</v>
-      </c>
-      <c r="F38" s="4" t="s">
-        <v>28</v>
-      </c>
-      <c r="G38" s="8">
-        <v>0.8958333333333334</v>
-      </c>
-      <c r="H38" s="4">
-        <v>1.0</v>
-      </c>
-      <c r="I38" s="4" t="s">
-        <v>7</v>
-      </c>
+      <c r="D38" s="9"/>
+      <c r="G38" s="6"/>
     </row>
     <row r="39">
       <c r="A39" s="1"/>

</xml_diff>

<commit_message>
rework update shedule, add remove session
</commit_message>
<xml_diff>
--- a/google/shedule.xlsx
+++ b/google/shedule.xlsx
@@ -11,7 +11,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="16">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="12">
   <si>
     <t>Расписание стримов</t>
   </si>
@@ -37,28 +37,16 @@
     <t>Озвучка/Сабы</t>
   </si>
   <si>
-    <t>304578501351047178</t>
-  </si>
-  <si>
-    <t>Деревенская глубинка 3</t>
-  </si>
-  <si>
-    <t>с 7 по 12</t>
+    <t>290166276796448768</t>
+  </si>
+  <si>
+    <t>TEST</t>
+  </si>
+  <si>
+    <t>с 1 по 6 (2 сезон)</t>
   </si>
   <si>
     <t>Субтитры</t>
-  </si>
-  <si>
-    <t>369138872048943115</t>
-  </si>
-  <si>
-    <t>Лагерь на свежем воздухе 2</t>
-  </si>
-  <si>
-    <t>с 1 по 6</t>
-  </si>
-  <si>
-    <t>Озвучка</t>
   </si>
 </sst>
 </file>
@@ -68,7 +56,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="d mmmm"/>
   </numFmts>
-  <fonts count="4">
+  <fonts count="5">
     <font>
       <sz val="10.0"/>
       <color rgb="FF000000"/>
@@ -78,6 +66,7 @@
       <color theme="1"/>
       <name val="Arial"/>
     </font>
+    <font/>
     <font>
       <sz val="10.0"/>
       <color rgb="FF112233"/>
@@ -108,7 +97,7 @@
   <cellStyleXfs count="1">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" applyAlignment="1" applyFont="1"/>
   </cellStyleXfs>
-  <cellXfs count="10">
+  <cellXfs count="13">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
     </xf>
@@ -124,19 +113,28 @@
     <xf borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0"/>
     </xf>
+    <xf borderId="0" fillId="0" fontId="2" numFmtId="164" xfId="0" applyAlignment="1" applyFont="1" applyNumberFormat="1">
+      <alignment readingOrder="0"/>
+    </xf>
+    <xf borderId="0" fillId="0" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment readingOrder="0"/>
+    </xf>
+    <xf borderId="0" fillId="0" fontId="2" numFmtId="20" xfId="0" applyAlignment="1" applyFont="1" applyNumberFormat="1">
+      <alignment readingOrder="0"/>
+    </xf>
     <xf borderId="0" fillId="0" fontId="1" numFmtId="164" xfId="0" applyAlignment="1" applyFont="1" applyNumberFormat="1">
       <alignment readingOrder="0"/>
     </xf>
+    <xf borderId="0" fillId="2" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyFill="1" applyFont="1">
+      <alignment readingOrder="0"/>
+    </xf>
     <xf borderId="0" fillId="0" fontId="1" numFmtId="20" xfId="0" applyAlignment="1" applyFont="1" applyNumberFormat="1">
-      <alignment readingOrder="0"/>
-    </xf>
-    <xf borderId="0" fillId="2" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyFill="1" applyFont="1">
       <alignment readingOrder="0"/>
     </xf>
     <xf borderId="0" fillId="0" fontId="1" numFmtId="164" xfId="0" applyAlignment="1" applyFont="1" applyNumberFormat="1">
       <alignment readingOrder="0" vertical="bottom"/>
     </xf>
-    <xf borderId="0" fillId="2" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+    <xf borderId="0" fillId="2" fontId="4" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0" vertical="bottom"/>
     </xf>
   </cellXfs>
@@ -404,22 +402,22 @@
     </row>
     <row r="4">
       <c r="B4" s="5">
-        <v>44295.0</v>
+        <v>44305.0</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" s="1"/>
-      <c r="D5" s="4" t="s">
+      <c r="D5" s="6" t="s">
         <v>8</v>
       </c>
-      <c r="E5" s="4" t="s">
+      <c r="E5" s="6" t="s">
         <v>9</v>
       </c>
-      <c r="F5" s="4" t="s">
+      <c r="F5" s="6" t="s">
         <v>10</v>
       </c>
-      <c r="G5" s="6">
-        <v>0.7916666666666666</v>
+      <c r="G5" s="7">
+        <v>0.875</v>
       </c>
       <c r="H5" s="4">
         <v>1.0</v>
@@ -433,57 +431,22 @@
     </row>
     <row r="7">
       <c r="A7" s="1"/>
-      <c r="B7" s="5">
-        <v>44296.0</v>
-      </c>
+      <c r="B7" s="5"/>
     </row>
     <row r="8">
       <c r="A8" s="1"/>
-      <c r="D8" s="4" t="s">
-        <v>12</v>
-      </c>
-      <c r="E8" s="4" t="s">
-        <v>13</v>
-      </c>
-      <c r="F8" s="4" t="s">
-        <v>14</v>
-      </c>
-      <c r="G8" s="6">
-        <v>0.625</v>
-      </c>
-      <c r="H8" s="4">
-        <v>1.0</v>
-      </c>
-      <c r="I8" s="4" t="s">
-        <v>15</v>
-      </c>
+      <c r="G8" s="7"/>
+    </row>
+    <row r="9">
+      <c r="G9" s="7"/>
     </row>
     <row r="10">
       <c r="A10" s="1"/>
-      <c r="B10" s="5">
-        <v>44297.0</v>
-      </c>
+      <c r="B10" s="5"/>
     </row>
     <row r="11">
       <c r="A11" s="1"/>
-      <c r="D11" s="4" t="s">
-        <v>12</v>
-      </c>
-      <c r="E11" s="4" t="s">
-        <v>13</v>
-      </c>
-      <c r="F11" s="4" t="s">
-        <v>10</v>
-      </c>
-      <c r="G11" s="6">
-        <v>0.625</v>
-      </c>
-      <c r="H11" s="4">
-        <v>1.0</v>
-      </c>
-      <c r="I11" s="4" t="s">
-        <v>15</v>
-      </c>
+      <c r="G11" s="7"/>
     </row>
     <row r="13">
       <c r="A13" s="1"/>
@@ -492,24 +455,24 @@
       <c r="A16" s="1"/>
     </row>
     <row r="18">
-      <c r="B18" s="5"/>
+      <c r="B18" s="8"/>
     </row>
     <row r="19">
       <c r="A19" s="1"/>
-      <c r="E19" s="7"/>
-      <c r="G19" s="6"/>
+      <c r="E19" s="9"/>
+      <c r="G19" s="10"/>
     </row>
     <row r="20">
       <c r="E20" s="2"/>
       <c r="F20" s="2"/>
     </row>
     <row r="21">
-      <c r="B21" s="5"/>
+      <c r="B21" s="8"/>
     </row>
     <row r="22">
       <c r="A22" s="1"/>
-      <c r="E22" s="7"/>
-      <c r="G22" s="6"/>
+      <c r="E22" s="9"/>
+      <c r="G22" s="10"/>
     </row>
     <row r="24">
       <c r="A24" s="1"/>
@@ -522,54 +485,54 @@
     </row>
     <row r="28">
       <c r="A28" s="1"/>
-      <c r="B28" s="8"/>
+      <c r="B28" s="11"/>
     </row>
     <row r="29">
       <c r="A29" s="1"/>
-      <c r="D29" s="9"/>
-      <c r="G29" s="6"/>
+      <c r="D29" s="12"/>
+      <c r="G29" s="10"/>
     </row>
     <row r="30">
-      <c r="B30" s="8"/>
-      <c r="D30" s="9"/>
-      <c r="G30" s="6"/>
+      <c r="B30" s="11"/>
+      <c r="D30" s="12"/>
+      <c r="G30" s="10"/>
     </row>
     <row r="31">
       <c r="A31" s="1"/>
-      <c r="B31" s="8"/>
+      <c r="B31" s="11"/>
       <c r="D31" s="1"/>
     </row>
     <row r="32">
       <c r="A32" s="1"/>
-      <c r="D32" s="9"/>
+      <c r="D32" s="12"/>
       <c r="F32" s="1"/>
-      <c r="G32" s="6"/>
+      <c r="G32" s="10"/>
     </row>
     <row r="33">
-      <c r="B33" s="8"/>
+      <c r="B33" s="11"/>
     </row>
     <row r="34">
       <c r="A34" s="1"/>
-      <c r="B34" s="8"/>
+      <c r="B34" s="11"/>
     </row>
     <row r="35">
-      <c r="D35" s="9"/>
-      <c r="G35" s="6"/>
+      <c r="D35" s="12"/>
+      <c r="G35" s="10"/>
     </row>
     <row r="36">
       <c r="A36" s="1"/>
-      <c r="D36" s="9"/>
-      <c r="G36" s="6"/>
+      <c r="D36" s="12"/>
+      <c r="G36" s="10"/>
     </row>
     <row r="37">
       <c r="A37" s="1"/>
-      <c r="B37" s="8"/>
+      <c r="B37" s="11"/>
       <c r="D37" s="2"/>
     </row>
     <row r="38">
       <c r="A38" s="1"/>
-      <c r="D38" s="9"/>
-      <c r="G38" s="6"/>
+      <c r="D38" s="12"/>
+      <c r="G38" s="10"/>
     </row>
     <row r="39">
       <c r="A39" s="1"/>

</xml_diff>